<commit_message>
Slight progress on understanding the CONT format.
</commit_message>
<xml_diff>
--- a/Panasonic CONT Format Reverse Engineering.xlsx
+++ b/Panasonic CONT Format Reverse Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Software\reverse-engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4B306-1D61-4924-B05C-8F749CFF8AD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F587011-DA94-448E-BDA1-B905090557C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C3DD6B92-908F-45C2-93AF-E8E034685CBA}"/>
   </bookViews>
@@ -20,6 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -295,9 +301,6 @@
     <t>0x04000021</t>
   </si>
   <si>
-    <t>These 4 bytes match the last four of the TMB and PMPD file data. They do not change when truncated by HD Writer.</t>
-  </si>
-  <si>
     <t>0x01000001</t>
   </si>
   <si>
@@ -335,7 +338,10 @@
     <t>This changes when truncating a file in HD Writer; last pair are sometimes NULs</t>
   </si>
   <si>
-    <t>This changes when truncating a file in HD Writer</t>
+    <t>These 4 bytes match the last four of the TMB and PMPD file data. They do not necessarily change when truncated by HD Writer. The last number seems to increase by 1 each year (i.e. 469 = 2019). The second last also changes with time (seems to remain the same if the minute is the same?)</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer. The latter 2 bytes seems to fluctuate around 256 (occasionally going above it). The first two bytes vary significantly.</t>
   </si>
 </sst>
 </file>
@@ -741,7 +747,7 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +755,7 @@
     <col min="1" max="1" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77" style="3" customWidth="1"/>
+    <col min="4" max="4" width="78.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
@@ -915,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>87</v>
@@ -937,10 +943,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,7 +957,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -962,7 +968,7 @@
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>101</v>
@@ -976,10 +982,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -990,10 +996,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1004,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,7 +1134,7 @@
         <v>28</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1156,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1181,7 @@
         <v>28</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,7 +1416,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>4</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>19</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,7 +1576,7 @@
         <v>33</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated notes on further investigation of unknown data fields.
</commit_message>
<xml_diff>
--- a/Panasonic CONT Format Reverse Engineering.xlsx
+++ b/Panasonic CONT Format Reverse Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Software\reverse-engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F587011-DA94-448E-BDA1-B905090557C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98208E59-9962-48C9-B15E-62735F4243B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C3DD6B92-908F-45C2-93AF-E8E034685CBA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
   <si>
     <t>Description</t>
   </si>
@@ -313,35 +313,64 @@
     <t>This seems to be constant between files and sources; possibly unused fields?</t>
   </si>
   <si>
-    <t>0x0101ef00 (before)
-0xeca3ee00 (after)</t>
-  </si>
-  <si>
-    <t>0x8012694a 0000 (before)
-0x807abd47 0000 (after)</t>
-  </si>
-  <si>
     <t>Video file size (in bytes)</t>
+  </si>
+  <si>
+    <t>This seems to be constant between files and sources (audio related?)</t>
+  </si>
+  <si>
+    <t>These 4 bytes match the last four of the TMB and PMPD file data. They do not necessarily change when truncated by HD Writer. The last number seems to increase by 1 each year (i.e. 469 = 2019). The second last also changes with time (seems to remain the same if the minute is the same?)</t>
+  </si>
+  <si>
+    <t>0x0101 (before)
+0xeca3 (after)</t>
+  </si>
+  <si>
+    <t>0xef00 (before)
+0xee00 (after)</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer. The values vary significantly.</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer. Most common value found was 240, but ranged between 145 and 261. Majority were between 239 and 245.</t>
+  </si>
+  <si>
+    <t>Constant regardless of source across all files examined.</t>
   </si>
   <si>
     <t>0x2000 (imported)
 0x2100 (project; single file)
+0x3000 (imported; previous version?)
 0x3100 (project; multiple clips)</t>
   </si>
   <si>
-    <t>This does not change when truncating a file in HD Writer, but does vary file to file. Might have to do with the origin of the video?</t>
-  </si>
-  <si>
-    <t>This seems to be constant between files and sources (audio related?)</t>
-  </si>
-  <si>
-    <t>This changes when truncating a file in HD Writer; last pair are sometimes NULs</t>
-  </si>
-  <si>
-    <t>These 4 bytes match the last four of the TMB and PMPD file data. They do not necessarily change when truncated by HD Writer. The last number seems to increase by 1 each year (i.e. 469 = 2019). The second last also changes with time (seems to remain the same if the minute is the same?)</t>
-  </si>
-  <si>
-    <t>This changes when truncating a file in HD Writer. The latter 2 bytes seems to fluctuate around 256 (occasionally going above it). The first two bytes vary significantly.</t>
+    <t>This does not change when truncating a file in HD Writer, but does vary file to file. Might have to do with the origin of the video? Have only seen four values and they seem to conform to a pattern.</t>
+  </si>
+  <si>
+    <t>0x8012 (before)
+0x807a (after)</t>
+  </si>
+  <si>
+    <t>0x694a (before)
+0xbd47 (after)</t>
+  </si>
+  <si>
+    <t>0x0000 (before)
+0x0000 (after)</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer. Almost always NULs, but occasionally they will be a small number (1-4 observed).</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer.</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer.
+2^0 through 2^6 always 0.
+2^7 typically 1; only observed to be 0 in HD Writer output (not consistent).
+2^8 typically 0; only observed to be 1 in HD Writer output (not consistent).
+2^9 through 2^15 have no observable pattern.</t>
   </si>
 </sst>
 </file>
@@ -744,17 +773,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D6A6B-C901-42E1-94D4-0C17B4653ADB}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="4"/>
   </cols>
@@ -921,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>87</v>
@@ -934,61 +963,64 @@
       <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>4</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>89</v>
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>2</v>
       </c>
@@ -999,54 +1031,60 @@
         <v>96</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>6</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>2</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>49</v>
+        <v>4</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>2</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>10</v>
+      <c r="B31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1054,7 +1092,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>10</v>
+        <v>49</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,13 +1106,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,7 +1114,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1084,13 +1128,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,7 +1136,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,13 +1150,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1120,21 +1158,21 @@
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>10</v>
+        <v>53</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>2</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>90</v>
+      <c r="B40" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,76 +1180,82 @@
         <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>10</v>
+        <v>69</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>2</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>98</v>
+      <c r="B42" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>2</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>70</v>
+      <c r="B43" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>71</v>
+        <v>28</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>2</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>98</v>
+      <c r="B44" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>2</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>10</v>
+      <c r="B45" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>2</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>74</v>
+      <c r="B47" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>56</v>
+        <v>28</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,21 +1263,18 @@
         <v>2</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,93 +1282,93 @@
         <v>2</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>10</v>
+        <v>74</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>4</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>67</v>
+        <v>2</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>256</v>
+        <v>2</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
+        <v>2</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>4</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
         <v>256</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="B55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>2</v>
+        <v>256</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>2</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
-        <v>14</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>8</v>
+      <c r="B58" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1335,12 +1376,32 @@
         <v>2</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>2</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="6" t="s">
-        <v>44</v>
+      <c r="A61" s="5">
+        <v>14</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1348,113 +1409,96 @@
         <v>2</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
-        <v>2</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
-        <v>2</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <v>4</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>4</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>100</v>
+      <c r="B69" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>78</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>2</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>9</v>
+      <c r="B71" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>4</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,12 +1506,29 @@
         <v>2</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>2</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="6" t="s">
-        <v>45</v>
+      <c r="A75" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1475,32 +1536,12 @@
         <v>2</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <v>2</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
-        <v>10</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>38</v>
+      <c r="B78" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,26 +1549,32 @@
         <v>2</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
-        <v>8</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
-        <v>2</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>78</v>
+        <v>10</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,18 +1585,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>13</v>
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>8</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,12 +1601,29 @@
         <v>2</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>2</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="6" t="s">
-        <v>46</v>
+      <c r="A86" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,32 +1631,12 @@
         <v>2</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
-        <v>2</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>8</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,7 +1644,13 @@
         <v>2</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>78</v>
+        <v>32</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,21 +1658,18 @@
         <v>2</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>8</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1633,32 +1677,62 @@
         <v>2</v>
       </c>
       <c r="B93" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>2</v>
+      </c>
+      <c r="B94" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="6" t="s">
-        <v>35</v>
+      <c r="A95" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
+        <v>2</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
         <v>16</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor changes, but still don't have a working output.
</commit_message>
<xml_diff>
--- a/Panasonic CONT Format Reverse Engineering.xlsx
+++ b/Panasonic CONT Format Reverse Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Software\reverse-engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98208E59-9962-48C9-B15E-62735F4243B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9C495A-4539-4836-B3E9-525C9D78CF26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C3DD6B92-908F-45C2-93AF-E8E034685CBA}"/>
   </bookViews>
@@ -363,14 +363,14 @@
     <t>This changes when truncating a file in HD Writer. Almost always NULs, but occasionally they will be a small number (1-4 observed).</t>
   </si>
   <si>
-    <t>This changes when truncating a file in HD Writer.</t>
+    <t>This changes when truncating a file in HD Writer. No pattern in the binary.</t>
   </si>
   <si>
     <t>This changes when truncating a file in HD Writer.
 2^0 through 2^6 always 0.
 2^7 typically 1; only observed to be 0 in HD Writer output (not consistent).
 2^8 typically 0; only observed to be 1 in HD Writer output (not consistent).
-2^9 through 2^15 have no observable pattern.</t>
+2^9 through 2^15 have no observable pattern. Independently each bit is set ~50% of the time.</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D6A6B-C901-42E1-94D4-0C17B4653ADB}">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Added ability to parse file creation dates.
</commit_message>
<xml_diff>
--- a/Panasonic CONT Format Reverse Engineering.xlsx
+++ b/Panasonic CONT Format Reverse Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Software\reverse-engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9C495A-4539-4836-B3E9-525C9D78CF26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15EF425-5E93-4D00-A69F-177B3752E458}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C3DD6B92-908F-45C2-93AF-E8E034685CBA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
   <si>
     <t>Description</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Consistent between files &amp; sources; perhaps this indicates the end of the header?</t>
   </si>
   <si>
-    <t>Length is consistent between file sources, but content differs (PMPD &amp; TMB data here is identical when output by HD Writer)</t>
-  </si>
-  <si>
     <t>File size (in bytes)</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
   </si>
   <si>
     <t>This seems to be constant between files and sources (audio related?)</t>
-  </si>
-  <si>
-    <t>These 4 bytes match the last four of the TMB and PMPD file data. They do not necessarily change when truncated by HD Writer. The last number seems to increase by 1 each year (i.e. 469 = 2019). The second last also changes with time (seems to remain the same if the minute is the same?)</t>
   </si>
   <si>
     <t>0x0101 (before)
@@ -371,6 +365,18 @@
 2^7 typically 1; only observed to be 0 in HD Writer output (not consistent).
 2^8 typically 0; only observed to be 1 in HD Writer output (not consistent).
 2^9 through 2^15 have no observable pattern. Independently each bit is set ~50% of the time.</t>
+  </si>
+  <si>
+    <t>Windows FILETIME value</t>
+  </si>
+  <si>
+    <t>Creation date of the TMB file</t>
+  </si>
+  <si>
+    <t>Creation date of the PMPD file</t>
+  </si>
+  <si>
+    <t>Creation date of the M2TS file</t>
   </si>
 </sst>
 </file>
@@ -773,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D6A6B-C901-42E1-94D4-0C17B4653ADB}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,10 +956,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,7 +970,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -975,10 +981,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -989,10 +995,10 @@
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1003,10 +1009,10 @@
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1017,7 +1023,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1028,10 +1034,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1042,10 +1048,10 @@
         <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1056,10 +1062,10 @@
         <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1070,10 +1076,10 @@
         <v>19</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1084,7 +1090,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1208,7 +1214,7 @@
         <v>28</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1236,7 @@
         <v>68</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,7 +1261,7 @@
         <v>28</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,7 +1332,7 @@
         <v>67</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>84</v>
@@ -1467,10 +1473,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1484,21 +1490,21 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>4</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
-        <v>4</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>95</v>
+        <v>2</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,42 +1512,48 @@
         <v>2</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
-        <v>2</v>
+      <c r="A74" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>39</v>
+      <c r="A75" s="5">
+        <v>2</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
-        <v>2</v>
-      </c>
-      <c r="B76" s="4" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="6" t="s">
-        <v>45</v>
+      <c r="A78" s="5">
+        <v>2</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1549,51 +1561,45 @@
         <v>2</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
-        <v>2</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
-        <v>10</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
-        <v>8</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,42 +1607,48 @@
         <v>2</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
-        <v>2</v>
+      <c r="A85" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>39</v>
+      <c r="A86" s="5">
+        <v>2</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
-        <v>2</v>
-      </c>
-      <c r="B87" s="4" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="6" t="s">
-        <v>46</v>
+      <c r="A89" s="5">
+        <v>2</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,32 +1656,26 @@
         <v>2</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
-        <v>8</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1677,62 +1683,54 @@
         <v>2</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
-        <v>2</v>
+      <c r="A94" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>2</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
-        <v>2</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>11</v>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
+      <c r="A98" s="5">
         <v>16</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Additional notes re TMB fields.
</commit_message>
<xml_diff>
--- a/Panasonic CONT Format Reverse Engineering.xlsx
+++ b/Panasonic CONT Format Reverse Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Software\reverse-engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15EF425-5E93-4D00-A69F-177B3752E458}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AC9283-ED9B-4531-962D-D82C7D940F14}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C3DD6B92-908F-45C2-93AF-E8E034685CBA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="115">
   <si>
     <t>Description</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>HD Writer Header Only</t>
-  </si>
-  <si>
-    <t>Length is consistent between file sources, but content differs</t>
   </si>
   <si>
     <t>Varies</t>
@@ -355,9 +352,6 @@
   </si>
   <si>
     <t>This changes when truncating a file in HD Writer. Almost always NULs, but occasionally they will be a small number (1-4 observed).</t>
-  </si>
-  <si>
-    <t>This changes when truncating a file in HD Writer. No pattern in the binary.</t>
   </si>
   <si>
     <t>This changes when truncating a file in HD Writer.
@@ -377,6 +371,24 @@
   </si>
   <si>
     <t>Creation date of the M2TS file</t>
+  </si>
+  <si>
+    <t>Note: video stream ID is 0x1011, but this doesn't seem to be in the CONT file</t>
+  </si>
+  <si>
+    <t>This changes when truncating a file in HD Writer. No obvious pattern in the binary.</t>
+  </si>
+  <si>
+    <t>0x5C03</t>
+  </si>
+  <si>
+    <t>Consistent between camera recordings (0x5c03), but varies from HD Writer. Last byte always 0x03, though.</t>
+  </si>
+  <si>
+    <t>0x9803</t>
+  </si>
+  <si>
+    <t>Consistent between camera recordings (0x9803), but varies from HD Writer. Last byte always 0x03, though.</t>
   </si>
 </sst>
 </file>
@@ -779,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D6A6B-C901-42E1-94D4-0C17B4653ADB}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,10 +822,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -824,13 +836,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,12 +883,15 @@
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,7 +907,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,7 +923,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,7 +955,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,10 +971,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,7 +985,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -981,10 +996,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -995,10 +1010,10 @@
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1009,10 +1024,10 @@
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1034,10 +1049,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1048,10 +1063,10 @@
         <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,10 +1077,10 @@
         <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1076,10 +1091,10 @@
         <v>19</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,7 +1105,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,13 +1113,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1120,13 +1135,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,13 +1157,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,13 +1179,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,13 +1201,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1208,13 +1223,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,13 +1245,13 @@
         <v>2</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,10 +1259,10 @@
         <v>2</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,13 +1270,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,10 +1292,10 @@
         <v>4</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,10 +1303,10 @@
         <v>2</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,7 +1314,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>30</v>
@@ -1310,10 +1325,10 @@
         <v>2</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,13 +1344,13 @@
         <v>4</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1435,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1449,7 @@
         <v>28</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,13 +1465,13 @@
         <v>2</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,10 +1488,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1493,10 +1508,10 @@
         <v>8</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1519,7 @@
         <v>2</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,7 +1532,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>4</v>
@@ -1539,7 +1554,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,15 +1579,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C80" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="D80" s="3" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1583,45 +1601,45 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
-        <v>8</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>107</v>
+        <v>2</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>10</v>
+        <v>105</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>39</v>
+      <c r="A85" s="5">
+        <v>2</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,45 +1647,48 @@
         <v>2</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>2</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>2</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
-        <v>2</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>10</v>
+      <c r="B90" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>107</v>
+        <v>32</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,29 +1696,26 @@
         <v>2</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>11</v>
+        <v>105</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>39</v>
+      <c r="A94" s="5">
+        <v>2</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1708,29 +1726,51 @@
         <v>11</v>
       </c>
     </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="6" t="s">
+      <c r="A97" s="5">
+        <v>2</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
         <v>16</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Partially worked out file duration...
</commit_message>
<xml_diff>
--- a/Panasonic CONT Format Reverse Engineering.xlsx
+++ b/Panasonic CONT Format Reverse Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Software\reverse-engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AC9283-ED9B-4531-962D-D82C7D940F14}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1956F1EF-C790-4292-8E2A-0E75B42340EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C3DD6B92-908F-45C2-93AF-E8E034685CBA}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Example</t>
   </si>
   <si>
-    <t>Datestamp DD.MM.YYYY (note zeroes in DD and MM are spaces)</t>
-  </si>
-  <si>
     <t>M2TS File Name</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
   </si>
   <si>
     <t>0x80BB</t>
-  </si>
-  <si>
-    <t>Length of filename (in bytes) (includes one pair of NUL bytes)</t>
   </si>
   <si>
     <t>Date of Recording</t>
@@ -376,9 +370,6 @@
     <t>Note: video stream ID is 0x1011, but this doesn't seem to be in the CONT file</t>
   </si>
   <si>
-    <t>This changes when truncating a file in HD Writer. No obvious pattern in the binary.</t>
-  </si>
-  <si>
     <t>0x5C03</t>
   </si>
   <si>
@@ -389,6 +380,17 @@
   </si>
   <si>
     <t>Consistent between camera recordings (0x9803), but varies from HD Writer. Last byte always 0x03, though.</t>
+  </si>
+  <si>
+    <t>Datestamp DD.MM.YYYY (zeroes in DD &amp; MM are spaces)</t>
+  </si>
+  <si>
+    <t>Length of filename in bytes (includes one pair of NUL bytes)</t>
+  </si>
+  <si>
+    <t>Video duration seems to be stored in the latter byte.
+Duration = (5/3)*(header value) + (4/3)
+Header value = 0.6*duration - 0.8</t>
   </si>
 </sst>
 </file>
@@ -793,22 +795,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D6A6B-C901-42E1-94D4-0C17B4653ADB}">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.7109375" style="3" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -822,13 +824,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +838,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,12 +855,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -866,13 +868,13 @@
         <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,18 +882,18 @@
         <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,7 +909,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,7 +941,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -947,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -955,7 +957,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -963,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,10 +973,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -982,10 +984,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -993,27 +995,27 @@
         <v>2</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1021,13 +1023,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,10 +1037,10 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1046,13 +1048,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1060,13 +1062,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,13 +1076,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1088,13 +1090,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1102,10 +1104,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,13 +1115,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,13 +1137,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1157,13 +1159,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,13 +1181,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1193,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1201,13 +1203,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,13 +1225,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,13 +1247,13 @@
         <v>2</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,10 +1261,10 @@
         <v>2</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,13 +1272,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1284,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1292,10 +1294,10 @@
         <v>4</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,10 +1305,10 @@
         <v>2</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,10 +1316,10 @@
         <v>2</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,10 +1327,10 @@
         <v>2</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1344,13 +1346,13 @@
         <v>4</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,13 +1360,13 @@
         <v>256</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,13 +1374,13 @@
         <v>256</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1386,10 +1388,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1397,10 +1399,10 @@
         <v>2</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,13 +1418,13 @@
         <v>14</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>3</v>
+        <v>112</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,12 +1432,12 @@
         <v>2</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,13 +1445,13 @@
         <v>2</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="D65" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1457,7 +1459,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1465,13 +1467,13 @@
         <v>2</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1479,7 +1481,7 @@
         <v>10</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C68" s="3"/>
     </row>
@@ -1488,10 +1490,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,7 +1501,7 @@
         <v>4</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C70" s="3"/>
     </row>
@@ -1508,10 +1510,10 @@
         <v>8</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1519,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,21 +1529,21 @@
         <v>2</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1549,12 +1551,12 @@
         <v>2</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,13 +1564,13 @@
         <v>2</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="D78" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1584,13 +1586,13 @@
         <v>2</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1598,7 +1600,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1606,13 +1608,13 @@
         <v>2</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,7 +1622,7 @@
         <v>6</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1628,10 +1630,10 @@
         <v>8</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1639,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,21 +1649,21 @@
         <v>2</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="D87" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1669,12 +1671,12 @@
         <v>2</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,13 +1684,13 @@
         <v>2</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="D91" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,7 +1698,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,10 +1706,10 @@
         <v>8</v>
       </c>
       <c r="B93" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,21 +1725,21 @@
         <v>2</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B96" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C96" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D96" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,12 +1747,12 @@
         <v>2</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,20 +1760,20 @@
         <v>16</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>